<commit_message>
Updated CSD util and testbase
</commit_message>
<xml_diff>
--- a/src/main/java/com/csd/testdata/CSD_TestData.xlsx
+++ b/src/main/java/com/csd/testdata/CSD_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15520" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15520" windowHeight="6950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +49,21 @@
   </si>
   <si>
     <t>CAH_TEST</t>
+  </si>
+  <si>
+    <t>IncName</t>
+  </si>
+  <si>
+    <t>contractName</t>
+  </si>
+  <si>
+    <t>LDAP is Down.This is a Test Incident</t>
+  </si>
+  <si>
+    <t>Sentinal is Down.This is a Test Incident</t>
+  </si>
+  <si>
+    <t>ES_TEST</t>
   </si>
 </sst>
 </file>
@@ -417,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -465,12 +480,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>